<commit_message>
sua loi fix nhan vien
</commit_message>
<xml_diff>
--- a/admin/qlnhanvien/DSnhanvien.xlsx
+++ b/admin/qlnhanvien/DSnhanvien.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
   <si>
     <t>DANH SÁCH NHÂN VIÊN TRUNG TÂM NGOẠI NGỮ AE</t>
   </si>
@@ -110,57 +110,54 @@
     <t>Kinh</t>
   </si>
   <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Xã An Hoà, huyện Ninh Kiều, tỉnh Cần Thơ</t>
+  </si>
+  <si>
+    <t>Long Xuyên</t>
+  </si>
+  <si>
+    <t>Nhân viên chính thức</t>
+  </si>
+  <si>
+    <t>Thạc sĩ</t>
+  </si>
+  <si>
+    <t>Bằng thạc sĩ</t>
+  </si>
+  <si>
+    <t>Kế Toán</t>
+  </si>
+  <si>
+    <t>Đang làm việc</t>
+  </si>
+  <si>
+    <t>MNVAE014</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Bé Gái</t>
+  </si>
+  <si>
+    <t>08/02/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An Giang </t>
+  </si>
+  <si>
+    <t>089097492841</t>
+  </si>
+  <si>
+    <t>24/06/2022</t>
+  </si>
+  <si>
+    <t>Cục Cảnh Sát An Giang</t>
+  </si>
+  <si>
     <t>Thiên Chúa Giáo</t>
   </si>
   <si>
-    <t>Xã An Hoà, huyện Ninh Kiều, tỉnh Cần Thơ</t>
-  </si>
-  <si>
-    <t>Long Xuyên</t>
-  </si>
-  <si>
-    <t>Nhân viên chính thức</t>
-  </si>
-  <si>
-    <t>Thạc sĩ</t>
-  </si>
-  <si>
-    <t>Không</t>
-  </si>
-  <si>
-    <t>Bằng thạc sĩ</t>
-  </si>
-  <si>
-    <t>Kế Toán</t>
-  </si>
-  <si>
-    <t>Đang làm việc</t>
-  </si>
-  <si>
-    <t>MNVAE014</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Bé Gái</t>
-  </si>
-  <si>
-    <t>08/02/2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An Giang </t>
-  </si>
-  <si>
-    <t>089097492841</t>
-  </si>
-  <si>
-    <t>24/06/2022</t>
-  </si>
-  <si>
-    <t>Cục Cảnh Sát An Giang</t>
-  </si>
-  <si>
-    <t>Phật Giáo</t>
-  </si>
-  <si>
     <t>Xã Phú Mỹ, huyện Châu Thành, tỉnh An Giang</t>
   </si>
   <si>
@@ -380,7 +377,7 @@
     <t>MNVAE004</t>
   </si>
   <si>
-    <t>Nguyễn Anh Đào</t>
+    <t>Võ Hoàng Anh Đào</t>
   </si>
   <si>
     <t>10/07/1999</t>
@@ -458,7 +455,7 @@
     <t>Giám đốc</t>
   </si>
   <si>
-    <t>Ngày xuất: 13/04/2024</t>
+    <t>Ngày xuất: 24/04/2024</t>
   </si>
 </sst>
 </file>
@@ -1023,16 +1020,16 @@
         <v>35</v>
       </c>
       <c r="Q3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -1040,28 +1037,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>29</v>
@@ -1070,10 +1067,10 @@
         <v>30</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>33</v>
@@ -1082,19 +1079,19 @@
         <v>34</v>
       </c>
       <c r="P4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="T4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -1102,61 +1099,61 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="T5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -1164,61 +1161,61 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="O6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="T6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -1226,61 +1223,61 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="T7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1288,40 +1285,40 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>33</v>
@@ -1333,16 +1330,16 @@
         <v>35</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1350,28 +1347,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>29</v>
@@ -1380,31 +1377,31 @@
         <v>30</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="O9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q9" s="4" t="s">
+      <c r="R9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="R9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="T9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1412,16 +1409,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>25</v>
@@ -1430,7 +1427,7 @@
         <v>896462371</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>28</v>
@@ -1439,34 +1436,34 @@
         <v>29</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="R10" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="S10" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1474,28 +1471,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="I11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>29</v>
@@ -1504,10 +1501,10 @@
         <v>30</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>33</v>
@@ -1516,19 +1513,19 @@
         <v>34</v>
       </c>
       <c r="P11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="T11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1536,61 +1533,61 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="G12" s="4">
         <v>892674672</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>33</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1598,40 +1595,40 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G13" s="4">
         <v>890874634</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>33</v>
@@ -1640,19 +1637,19 @@
         <v>34</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1660,28 +1657,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="I14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>29</v>
@@ -1690,10 +1687,10 @@
         <v>30</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>33</v>
@@ -1702,19 +1699,19 @@
         <v>34</v>
       </c>
       <c r="P14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" s="4" t="s">
+      <c r="R14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="R14" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="S14" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1722,28 +1719,28 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="I15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>29</v>
@@ -1752,10 +1749,10 @@
         <v>30</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>33</v>
@@ -1764,19 +1761,19 @@
         <v>34</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1784,28 +1781,28 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="I16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>29</v>
@@ -1814,10 +1811,10 @@
         <v>30</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>33</v>
@@ -1829,16 +1826,16 @@
         <v>35</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1846,28 +1843,28 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="I17" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>29</v>
@@ -1876,10 +1873,10 @@
         <v>30</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>33</v>
@@ -1891,21 +1888,21 @@
         <v>35</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>